<commit_message>
Initial version of Cards_Treasures.xlsx added
</commit_message>
<xml_diff>
--- a/projecting/cards_treasures.xlsx
+++ b/projecting/cards_treasures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="184">
   <si>
     <t>CardId</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Hammer of Kneecapping</t>
   </si>
   <si>
-    <t>Hireling</t>
-  </si>
-  <si>
     <t>Transferral Potion</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>Cheese Grater of Peace</t>
   </si>
   <si>
-    <t>Loaded Die</t>
-  </si>
-  <si>
     <t>Nasty-Tasting Sports Drink</t>
   </si>
   <si>
@@ -288,6 +282,300 @@
   </si>
   <si>
     <t>Eleven-Foot Pole</t>
+  </si>
+  <si>
+    <t>Baby Oil</t>
+  </si>
+  <si>
+    <t>Your Shoe's Untied!</t>
+  </si>
+  <si>
+    <t>Raincoat</t>
+  </si>
+  <si>
+    <t>Potion of Cowardice</t>
+  </si>
+  <si>
+    <t>Loaded Die_2</t>
+  </si>
+  <si>
+    <t>Loaded Die_1</t>
+  </si>
+  <si>
+    <t>Potion of Flight</t>
+  </si>
+  <si>
+    <t>…Of Doom!</t>
+  </si>
+  <si>
+    <t>armorAmplifier</t>
+  </si>
+  <si>
+    <t>Itching Powder</t>
+  </si>
+  <si>
+    <t>Tweezers of Terror</t>
+  </si>
+  <si>
+    <t>Cute Shoulder Dragon</t>
+  </si>
+  <si>
+    <t>Fold, Spindle, and Mutilate</t>
+  </si>
+  <si>
+    <t>Promise the GM You'll Stop Telling Him About Your Character</t>
+  </si>
+  <si>
+    <t>Trojan Horse</t>
+  </si>
+  <si>
+    <t>Lemming Juice</t>
+  </si>
+  <si>
+    <t>Unnatural Axe</t>
+  </si>
+  <si>
+    <t>Druid Fluid</t>
+  </si>
+  <si>
+    <t>Slug Thrower</t>
+  </si>
+  <si>
+    <t>Boomdagger</t>
+  </si>
+  <si>
+    <t>Coat of Arms</t>
+  </si>
+  <si>
+    <t>Bag of Caltrops</t>
+  </si>
+  <si>
+    <t>Contemplate Your Navel</t>
+  </si>
+  <si>
+    <t>Barbecue Fork</t>
+  </si>
+  <si>
+    <t>Blessed Mallet of St. Eeeeeeuuuuuuuuw</t>
+  </si>
+  <si>
+    <t>Very Holy Book</t>
+  </si>
+  <si>
+    <t>Big Thing</t>
+  </si>
+  <si>
+    <t>Funny-Looking Sword</t>
+  </si>
+  <si>
+    <t>Tinfoil Hat</t>
+  </si>
+  <si>
+    <t>Loaded Die_3</t>
+  </si>
+  <si>
+    <t>Potion of Disbelief</t>
+  </si>
+  <si>
+    <t>Lawn Roller</t>
+  </si>
+  <si>
+    <t>Helm of Peripheral Vision</t>
+  </si>
+  <si>
+    <t>Knight Light</t>
+  </si>
+  <si>
+    <t>Spiked Codpiece</t>
+  </si>
+  <si>
+    <t>Pay For The Pizza</t>
+  </si>
+  <si>
+    <t>Switch Character Sheets</t>
+  </si>
+  <si>
+    <t>Sword of Slaying Everything Except Squid</t>
+  </si>
+  <si>
+    <t>Fake Beard</t>
+  </si>
+  <si>
+    <t>Familiar</t>
+  </si>
+  <si>
+    <t>Wash The GM's Car</t>
+  </si>
+  <si>
+    <t>Siege Engine</t>
+  </si>
+  <si>
+    <t>Skull Helmet</t>
+  </si>
+  <si>
+    <t>Blac-hair Girl Mage with staff</t>
+  </si>
+  <si>
+    <t>Garage Sale</t>
+  </si>
+  <si>
+    <t>Scary False Teeth</t>
+  </si>
+  <si>
+    <t>Unnecessary Roughness</t>
+  </si>
+  <si>
+    <t>Wishing Ring_3</t>
+  </si>
+  <si>
+    <t>Stab-A-Matic</t>
+  </si>
+  <si>
+    <t>WildAxe</t>
+  </si>
+  <si>
+    <t>The Occasionally Reliable Amulet</t>
+  </si>
+  <si>
+    <t>Fake Ears</t>
+  </si>
+  <si>
+    <t>Remember The GM's Birthday</t>
+  </si>
+  <si>
+    <t>Take Me! Take Me!</t>
+  </si>
+  <si>
+    <t>Threaten To Switch Systems</t>
+  </si>
+  <si>
+    <t>Tasty Pie</t>
+  </si>
+  <si>
+    <t>The Dungeon Casino</t>
+  </si>
+  <si>
+    <t>The Other Ring</t>
+  </si>
+  <si>
+    <t>Vorpal Blade</t>
+  </si>
+  <si>
+    <t>Potion of Apathy</t>
+  </si>
+  <si>
+    <t>Hot Pepper Sauce</t>
+  </si>
+  <si>
+    <t>Feline Intervention</t>
+  </si>
+  <si>
+    <t>Illustrate Your Character</t>
+  </si>
+  <si>
+    <t>Gnomex Suit</t>
+  </si>
+  <si>
+    <t>Steal The Credit</t>
+  </si>
+  <si>
+    <t>Semi-Final Strike</t>
+  </si>
+  <si>
+    <t>Dwarf Tossing</t>
+  </si>
+  <si>
+    <t>Castig Couch</t>
+  </si>
+  <si>
+    <t>Chainmail Bikini</t>
+  </si>
+  <si>
+    <t>Magnificent Hat</t>
+  </si>
+  <si>
+    <t>Rewrite That Dirty Old Character Sheet</t>
+  </si>
+  <si>
+    <t>Deus Ex Machinegun</t>
+  </si>
+  <si>
+    <t>Royal Oil</t>
+  </si>
+  <si>
+    <t>One Size Fits All</t>
+  </si>
+  <si>
+    <t>Wishing Ring_4</t>
+  </si>
+  <si>
+    <t>Slay Bells</t>
+  </si>
+  <si>
+    <t>Freudian Slippers</t>
+  </si>
+  <si>
+    <t>Duck of Many Things</t>
+  </si>
+  <si>
+    <t>Two-Handed Sword</t>
+  </si>
+  <si>
+    <t>Blessed</t>
+  </si>
+  <si>
+    <t>Restraining Order</t>
+  </si>
+  <si>
+    <t>Joy Buzzer</t>
+  </si>
+  <si>
+    <t>Poisoned</t>
+  </si>
+  <si>
+    <t>Monster Chow</t>
+  </si>
+  <si>
+    <t>Loaded Die_4</t>
+  </si>
+  <si>
+    <t>Liquid Wench</t>
+  </si>
+  <si>
+    <t>Convenient Handles</t>
+  </si>
+  <si>
+    <t>Big Fat Lyre</t>
+  </si>
+  <si>
+    <t>Oil of Boiling</t>
+  </si>
+  <si>
+    <t>Foot-Mounted Mace</t>
+  </si>
+  <si>
+    <t>Senseless Act Of Kindness</t>
+  </si>
+  <si>
+    <t>Shiny Dice… Spinning… Spinning…</t>
+  </si>
+  <si>
+    <t>Hireling_2</t>
+  </si>
+  <si>
+    <t>Girl</t>
+  </si>
+  <si>
+    <t>Hireling_1</t>
+  </si>
+  <si>
+    <t>Ghoul Lash</t>
+  </si>
+  <si>
+    <t>Awful Socks</t>
+  </si>
+  <si>
+    <t>ClericalErrors</t>
   </si>
 </sst>
 </file>
@@ -643,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119:D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +942,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -1047,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>180</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -1065,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -1083,7 +1371,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -1101,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -1119,7 +1407,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -1137,7 +1425,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
@@ -1155,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -1173,7 +1461,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
@@ -1191,7 +1479,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
@@ -1209,7 +1497,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
@@ -1227,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
@@ -1245,7 +1533,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
@@ -1263,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
@@ -1281,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
@@ -1299,7 +1587,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
@@ -1317,7 +1605,7 @@
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
@@ -1335,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
@@ -1353,7 +1641,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
@@ -1371,7 +1659,7 @@
         <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
@@ -1389,7 +1677,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
@@ -1407,7 +1695,7 @@
         <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
@@ -1425,7 +1713,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>8</v>
@@ -1443,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>8</v>
@@ -1461,7 +1749,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>8</v>
@@ -1479,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>8</v>
@@ -1497,7 +1785,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
@@ -1515,7 +1803,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -1533,7 +1821,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
@@ -1551,7 +1839,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>8</v>
@@ -1569,7 +1857,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
@@ -1587,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -1605,7 +1893,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
@@ -1623,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
@@ -1641,7 +1929,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -1659,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
@@ -1677,7 +1965,7 @@
         <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>8</v>
@@ -1695,7 +1983,7 @@
         <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
@@ -1713,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
@@ -1731,7 +2019,7 @@
         <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
@@ -1749,7 +2037,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
@@ -1767,7 +2055,7 @@
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>8</v>
@@ -1785,7 +2073,7 @@
         <v>6</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>8</v>
@@ -1803,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>8</v>
@@ -1821,7 +2109,7 @@
         <v>6</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
@@ -1839,7 +2127,7 @@
         <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>8</v>
@@ -1857,7 +2145,7 @@
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>8</v>
@@ -1875,7 +2163,7 @@
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>8</v>
@@ -1886,14 +2174,14 @@
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" ref="A69:A74" si="1">A68+1</f>
+        <f t="shared" ref="A69:A132" si="1">A68+1</f>
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>8</v>
@@ -1911,13 +2199,13 @@
         <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>30</v>
@@ -1932,7 +2220,7 @@
         <v>6</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -1950,7 +2238,7 @@
         <v>6</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -1968,7 +2256,7 @@
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -1986,13 +2274,1369 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <f t="shared" ref="A133:A164" si="2">A132+1</f>
+        <v>132</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial tables modified, new added.
-Doors modified (to check - everything was Ok)
-Treasures modified (with respect to classes)
-Treasures-armor Table added (initial)
</commit_message>
<xml_diff>
--- a/projecting/cards_treasures.xlsx
+++ b/projecting/cards_treasures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="183">
   <si>
     <t>CardId</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Spiky Knees</t>
   </si>
   <si>
-    <t>SmallThing</t>
-  </si>
-  <si>
     <t>Pretty Balloons</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Shield of Ubiquity</t>
   </si>
   <si>
-    <t>Multilate the Bodies</t>
-  </si>
-  <si>
     <t>Whine at the GM</t>
   </si>
   <si>
@@ -362,9 +356,6 @@
     <t>Very Holy Book</t>
   </si>
   <si>
-    <t>Big Thing</t>
-  </si>
-  <si>
     <t>Funny-Looking Sword</t>
   </si>
   <si>
@@ -576,6 +567,12 @@
   </si>
   <si>
     <t>ClericalErrors</t>
+  </si>
+  <si>
+    <t>ThingAmplifier</t>
+  </si>
+  <si>
+    <t>Mutilate the Bodies</t>
   </si>
 </sst>
 </file>
@@ -933,14 +930,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:D164"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F71" sqref="F49:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
@@ -987,13 +984,14 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1011,43 +1009,43 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A68" si="0">A4+1</f>
+        <f>A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f>A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1058,86 +1056,86 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f>A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f>A7+1</f>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f>A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f>A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f>A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -1148,32 +1146,32 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f>A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f>A12+1</f>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1184,71 +1182,71 @@
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f>A13+1</f>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f>A14+1</f>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f>A15+1</f>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f>A16+1</f>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>116</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1256,2390 +1254,2662 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f>A17+1</f>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f>A18+1</f>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f>A19+1</f>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f>A20+1</f>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>152</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f>A21+1</f>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f>A22+1</f>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
+        <f>A23+1</f>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
+        <f>A24+1</f>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" si="0"/>
+        <f>A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>165</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
+        <f>A26+1</f>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>169</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f>A28+1</f>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f>A29+1</f>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>A30+1</f>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f>A31+1</f>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>A32+1</f>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f>A33+1</f>
+        <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <f>A34+1</f>
+        <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>A35+1</f>
+        <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>A36+1</f>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>A37+1</f>
+        <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f>A38+1</f>
+        <v>13</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>A39+1</f>
+        <v>14</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>A40+1</f>
+        <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <f>A41+1</f>
+        <v>16</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>A42+1</f>
+        <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <f>A43+1</f>
+        <v>18</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <f>A44+1</f>
+        <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>A45+1</f>
+        <v>20</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <f>A46+1</f>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <f>A47+1</f>
+        <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <f>A48+1</f>
+        <v>23</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>A49+1</f>
+        <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f>A50+1</f>
+        <v>25</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <f t="shared" si="0"/>
+        <f>A51+1</f>
+        <v>26</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>A52+1</f>
+        <v>27</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>63</v>
+        <v>182</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>A53+1</f>
+        <v>28</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <f>A54+1</f>
+        <v>29</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <f>A55+1</f>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f>A56+1</f>
+        <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f>A57+1</f>
+        <v>32</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <f>A58+1</f>
+        <v>33</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <f>A59+1</f>
+        <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <f>A60+1</f>
+        <v>35</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <f>A61+1</f>
+        <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <f>A62+1</f>
+        <v>37</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <f>A63+1</f>
+        <v>38</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <f>A64+1</f>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f>A65+1</f>
+        <v>40</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <f t="shared" si="0"/>
-        <v>66</v>
+        <f>A66+1</f>
+        <v>41</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" si="0"/>
-        <v>67</v>
+        <f>A67+1</f>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" ref="A69:A132" si="1">A68+1</f>
-        <v>68</v>
+        <f>A68+1</f>
+        <v>43</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="1"/>
-        <v>69</v>
+        <f>A69+1</f>
+        <v>44</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>79</v>
+        <v>180</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f>A70+1</f>
+        <v>45</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <f>A71+1</f>
+        <v>46</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="1"/>
-        <v>72</v>
+        <f>A72+1</f>
+        <v>47</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="1"/>
-        <v>73</v>
+        <f>A73+1</f>
+        <v>48</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="1"/>
+        <f>A74+1</f>
+        <v>49</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <f>A75+1</f>
+        <v>50</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <f>A76+1</f>
+        <v>51</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <f>A77+1</f>
+        <v>52</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f>A78+1</f>
+        <v>53</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <f>A79+1</f>
+        <v>54</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <f>A80+1</f>
+        <v>55</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <f>A81+1</f>
+        <v>56</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <f>A82+1</f>
+        <v>57</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <f>A83+1</f>
+        <v>58</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D84" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="1"/>
+        <f>A84+1</f>
+        <v>59</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <f>A85+1</f>
+        <v>60</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <f>A86+1</f>
+        <v>61</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D87" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <f>A87+1</f>
+        <v>62</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f>A88+1</f>
+        <v>63</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f>A89+1</f>
+        <v>64</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <f>A90+1</f>
+        <v>65</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D91" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="1"/>
-        <v>91</v>
+        <f>A91+1</f>
+        <v>66</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="1"/>
-        <v>92</v>
+        <f>A92+1</f>
+        <v>67</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="1"/>
-        <v>93</v>
+        <f>A93+1</f>
+        <v>68</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="1"/>
-        <v>94</v>
+        <f>A94+1</f>
+        <v>69</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f t="shared" si="1"/>
-        <v>95</v>
+        <f>A95+1</f>
+        <v>70</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f t="shared" si="1"/>
-        <v>96</v>
+        <f>A96+1</f>
+        <v>71</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f t="shared" si="1"/>
-        <v>97</v>
+        <f>A97+1</f>
+        <v>72</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f t="shared" si="1"/>
-        <v>98</v>
+        <f>A98+1</f>
+        <v>73</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f t="shared" si="1"/>
-        <v>99</v>
+        <f>A99+1</f>
+        <v>74</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>A100+1</f>
+        <v>75</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <f t="shared" si="1"/>
-        <v>101</v>
+        <f>A101+1</f>
+        <v>76</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <f t="shared" si="1"/>
-        <v>102</v>
+        <f>A102+1</f>
+        <v>77</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <f t="shared" si="1"/>
-        <v>103</v>
+        <f>A103+1</f>
+        <v>78</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <f t="shared" si="1"/>
-        <v>104</v>
+        <f>A104+1</f>
+        <v>79</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <f t="shared" si="1"/>
-        <v>105</v>
+        <f>A105+1</f>
+        <v>80</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <f t="shared" si="1"/>
-        <v>106</v>
+        <f>A106+1</f>
+        <v>81</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <f t="shared" si="1"/>
-        <v>107</v>
+        <f>A107+1</f>
+        <v>82</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <f t="shared" si="1"/>
-        <v>108</v>
+        <f>A108+1</f>
+        <v>83</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <f t="shared" si="1"/>
-        <v>109</v>
+        <f>A109+1</f>
+        <v>84</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <f t="shared" si="1"/>
-        <v>110</v>
+        <f>A110+1</f>
+        <v>85</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <f t="shared" si="1"/>
-        <v>111</v>
+        <f>A111+1</f>
+        <v>86</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <f t="shared" si="1"/>
-        <v>112</v>
+        <f>A112+1</f>
+        <v>87</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <f t="shared" si="1"/>
-        <v>113</v>
+        <f>A113+1</f>
+        <v>88</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <f t="shared" si="1"/>
-        <v>114</v>
+        <f>A114+1</f>
+        <v>89</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <f t="shared" si="1"/>
-        <v>115</v>
+        <f>A115+1</f>
+        <v>90</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <f t="shared" si="1"/>
-        <v>116</v>
+        <f>A116+1</f>
+        <v>91</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <f t="shared" si="1"/>
-        <v>117</v>
+        <f>A117+1</f>
+        <v>92</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <f t="shared" si="1"/>
-        <v>118</v>
+        <f>A118+1</f>
+        <v>93</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>25</v>
+        <v>181</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <f t="shared" si="1"/>
-        <v>119</v>
+        <f>A119+1</f>
+        <v>94</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>A120+1</f>
+        <v>95</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <f t="shared" si="1"/>
+        <f>A121+1</f>
+        <v>96</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <f t="shared" si="1"/>
+        <f>A122+1</f>
+        <v>97</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D123" s="1" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>30</v>
+        <v>181</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <f t="shared" si="1"/>
-        <v>123</v>
+        <f>A123+1</f>
+        <v>98</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <f>A124+1</f>
+        <v>99</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <f>A125+1</f>
+        <v>100</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <f>A126+1</f>
+        <v>101</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <f t="shared" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="D127" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <f t="shared" si="1"/>
-        <v>127</v>
+        <f>A127+1</f>
+        <v>102</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F128" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <f>A128+1</f>
+        <v>103</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <f>A129+1</f>
+        <v>104</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <f>A130+1</f>
+        <v>105</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <f t="shared" si="1"/>
-        <v>128</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <f t="shared" si="1"/>
-        <v>129</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="D131" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <f t="shared" si="1"/>
-        <v>131</v>
+        <f>A131+1</f>
+        <v>106</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <f t="shared" ref="A133:A164" si="2">A132+1</f>
-        <v>132</v>
+        <f>A132+1</f>
+        <v>107</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <f t="shared" si="2"/>
-        <v>133</v>
+        <f>A133+1</f>
+        <v>108</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>150</v>
+        <v>31</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <f t="shared" si="2"/>
-        <v>134</v>
+        <f>A134+1</f>
+        <v>109</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <f t="shared" si="2"/>
-        <v>135</v>
+        <f>A135+1</f>
+        <v>110</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <f t="shared" si="2"/>
-        <v>136</v>
+        <f>A136+1</f>
+        <v>111</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F137" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <f>A137+1</f>
         <v>112</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <f t="shared" si="2"/>
-        <v>137</v>
+      <c r="B138" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <f t="shared" si="2"/>
-        <v>138</v>
+        <f>A138+1</f>
+        <v>113</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>155</v>
+        <v>46</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <f t="shared" si="2"/>
-        <v>139</v>
+        <f>A139+1</f>
+        <v>114</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>156</v>
+        <v>50</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <f t="shared" si="2"/>
-        <v>140</v>
+        <f>A140+1</f>
+        <v>115</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <f t="shared" si="2"/>
+        <f>A141+1</f>
+        <v>116</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <f>A142+1</f>
+        <v>117</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <f>A143+1</f>
+        <v>118</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <f>A144+1</f>
+        <v>119</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <f>A145+1</f>
+        <v>120</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <f>A146+1</f>
+        <v>121</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <f>A147+1</f>
+        <v>122</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <f>A148+1</f>
+        <v>123</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <f>A149+1</f>
+        <v>124</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <f>A150+1</f>
+        <v>125</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <f>A151+1</f>
+        <v>126</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <f>A152+1</f>
+        <v>127</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <f>A153+1</f>
+        <v>128</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <f>A154+1</f>
+        <v>129</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <f>A155+1</f>
+        <v>130</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <f>A156+1</f>
+        <v>131</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <f>A157+1</f>
+        <v>132</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <f>A158+1</f>
+        <v>133</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <f t="shared" si="2"/>
-        <v>142</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <f t="shared" si="2"/>
-        <v>143</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <f t="shared" si="2"/>
-        <v>144</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <f t="shared" si="2"/>
-        <v>146</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <f t="shared" si="2"/>
-        <v>149</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
-        <f t="shared" si="2"/>
-        <v>151</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <f t="shared" si="2"/>
-        <v>152</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <f t="shared" si="2"/>
-        <v>153</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <f t="shared" si="2"/>
-        <v>154</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <f t="shared" si="2"/>
-        <v>155</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <f t="shared" si="2"/>
-        <v>156</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <f t="shared" si="2"/>
-        <v>157</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <f t="shared" si="2"/>
-        <v>158</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="D159" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <f t="shared" si="2"/>
-        <v>159</v>
+        <f>A159+1</f>
+        <v>134</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f>A160+1</f>
+        <v>135</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <f t="shared" si="2"/>
-        <v>161</v>
+        <f>A161+1</f>
+        <v>136</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C162" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <f>A162+1</f>
+        <v>137</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <f>A163+1</f>
+        <v>138</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <f t="shared" si="2"/>
-        <v>162</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <f t="shared" si="2"/>
-        <v>163</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="D164" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F164">
+    <sortCondition ref="F1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>